<commit_message>
anonymized data for demo
</commit_message>
<xml_diff>
--- a/public/risk.xlsx
+++ b/public/risk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WesleyPowell\OneDrive - Scout Motors Inc\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06CDA04-1261-4A60-9B6D-4F0FE41A9467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EE0D77-2297-4496-AEBC-4462D3D76424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5CE9F47-AF3C-47FC-B770-689BF2460523}"/>
   </bookViews>
@@ -36,34 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
-  <si>
-    <t>Material costs worsen from May 2025 K-VAP status (VSI)</t>
-  </si>
-  <si>
-    <t>Target sales and service model not viable</t>
-  </si>
-  <si>
-    <t>Tariff risks on MEK from CAN, MEX, and EU sourcing</t>
-  </si>
-  <si>
-    <t>Tariff risks on production equipment and supplier tooling</t>
-  </si>
-  <si>
-    <t>Localization costs for LK4 and EA211 FSI</t>
-  </si>
-  <si>
-    <t>Lafrentz / Adam</t>
-  </si>
-  <si>
-    <t>Thacker / Sitron</t>
-  </si>
-  <si>
-    <t>Kodumudi</t>
-  </si>
-  <si>
-    <t>Kodumudi / Wollinsky</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>2027 - 2040</t>
   </si>
@@ -104,40 +77,64 @@
     <t>Date Added</t>
   </si>
   <si>
-    <t>$997 material cost decrease: $42,950 May 
-2025 K-VAP VSI vs $41,953 Aug. 2025 
-interim status; Unrealized risk of $2,536 identified</t>
-  </si>
-  <si>
-    <t>Vehicle revenue loss from MSRP % paid to 
-dealer; Loss of incremental revenues (parts, service, accessories, connectivity, and others; Other incremental costs (higher warranty 
-cost provision, corporate OpEx, IT)</t>
-  </si>
-  <si>
-    <t>EA211: $157.3M initial invest + $57.7M for
-Silao expansion risk; LK4: $418.3M initial invest + $26.6M structure</t>
-  </si>
-  <si>
-    <t>LK4 imports from EU→Mexico; Non-USMCA 
-compliant EDU assemblies; 15% duty on imported CKD components from EU' Battery cell imports for 2028 and early  2029</t>
-  </si>
-  <si>
-    <t>Equipment tariff and forex risk: $89.6M</t>
-  </si>
-  <si>
-    <t>Material cost VSI improved since May 2025 K-VAP status due to Cost Sprint efforts; Risk identified in major components such as the battery pack based on supplier offers, LK4 prices, pre-assemblies and LV harnesses</t>
-  </si>
-  <si>
-    <t>Achieved licenses necessary to preserve go_x0002_to-market optionality in California, Missouri, Illinois, Utah – enabling 50-state direct sales; Arizona and Colorado license application underway, licenses expected Q3-Q4 2025; ~47 states open for direct service</t>
-  </si>
-  <si>
-    <t>Scout included invest in PR74.OP submission until agreement made by Group how funds should be accounted across Brands</t>
-  </si>
-  <si>
-    <t>Updated tariffs on imported auto parts from EU to 15; Consider non-USMCA tariff risk of 27.5% on FR/RR EDUs w/Audi LK4 imports</t>
-  </si>
-  <si>
-    <t>Risk considers NPV time effects</t>
+    <t>Risk A</t>
+  </si>
+  <si>
+    <t>Risk B</t>
+  </si>
+  <si>
+    <t>Risk C</t>
+  </si>
+  <si>
+    <t>Risk D</t>
+  </si>
+  <si>
+    <t>Risk E</t>
+  </si>
+  <si>
+    <t>Responsible A</t>
+  </si>
+  <si>
+    <t>Responsible B</t>
+  </si>
+  <si>
+    <t>Responsible C</t>
+  </si>
+  <si>
+    <t>Responsible D</t>
+  </si>
+  <si>
+    <t>Responsible E</t>
+  </si>
+  <si>
+    <t>Calculation A</t>
+  </si>
+  <si>
+    <t>Calculation B</t>
+  </si>
+  <si>
+    <t>Calculation C</t>
+  </si>
+  <si>
+    <t>Calculation D</t>
+  </si>
+  <si>
+    <t>Calculation E</t>
+  </si>
+  <si>
+    <t>Update A</t>
+  </si>
+  <si>
+    <t>Update B</t>
+  </si>
+  <si>
+    <t>Update C</t>
+  </si>
+  <si>
+    <t>Update D</t>
+  </si>
+  <si>
+    <t>Update E</t>
   </si>
 </sst>
 </file>
@@ -209,7 +206,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -218,18 +215,6 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -244,6 +229,18 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -276,18 +273,18 @@
   <autoFilter ref="A1:I6" xr:uid="{D55D8DBA-8FB4-4C67-9F9E-6DF313724C5F}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BF13F786-4B04-4961-A30B-78983255055B}" name="Risk Name" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{B5D08A0D-A40D-4276-BB27-E84F502AEF02}" name="Total Impact" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{B5D08A0D-A40D-4276-BB27-E84F502AEF02}" name="Total Impact" dataDxfId="7">
       <calculatedColumnFormula>-1281*1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{86BAB539-FD29-458F-B3C8-CA75E2D5E24F}" name="Likelihood" dataDxfId="0" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{44AB7870-F2B8-40F2-9B61-8A9C041484F9}" name="Risk by Likelihood" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{86BAB539-FD29-458F-B3C8-CA75E2D5E24F}" name="Likelihood" dataDxfId="6" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{44AB7870-F2B8-40F2-9B61-8A9C041484F9}" name="Risk by Likelihood" dataDxfId="5">
       <calculatedColumnFormula>Table1[[#This Row],[Total Impact]]*Table1[[#This Row],[Likelihood]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{185EE216-6CE0-4433-8B49-A3D0EF80E5DE}" name="Responsible" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{2673E1ED-1064-4E6C-ABF7-D939B3437712}" name="Impact Years" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{CC3C2859-EFDE-405F-844A-58250EDF07DD}" name="Calculation Basis" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{B990CD74-FE9D-48EB-8B0D-51088C7BFC33}" name="Updates" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{43A2270C-CC3B-498C-9C65-628DB63036D8}" name="Date Added" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{185EE216-6CE0-4433-8B49-A3D0EF80E5DE}" name="Responsible" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{2673E1ED-1064-4E6C-ABF7-D939B3437712}" name="Impact Years" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{CC3C2859-EFDE-405F-844A-58250EDF07DD}" name="Calculation Basis" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{B990CD74-FE9D-48EB-8B0D-51088C7BFC33}" name="Updates" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{43A2270C-CC3B-498C-9C65-628DB63036D8}" name="Date Added" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -613,55 +610,55 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="46.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.109375" style="1"/>
+    <col min="7" max="7" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="46.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="B2" s="3">
         <f>1281*1000000</f>
@@ -675,24 +672,24 @@
         <v>108885000000</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I2" s="4">
         <v>45839</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3">
         <f>8700*1000000</f>
@@ -706,55 +703,55 @@
         <v>130500000000</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I3" s="4">
         <v>45839</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3">
         <f>536*1000000</f>
         <v>536000000</v>
       </c>
       <c r="C4" s="6">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="D4" s="3">
         <f>Table1[[#This Row],[Total Impact]]*Table1[[#This Row],[Likelihood]]</f>
-        <v>536000000</v>
+        <v>53600000000</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I4" s="4">
         <v>45839</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3">
         <f>382*1000000</f>
@@ -768,16 +765,16 @@
         <v>3056000000</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I5" s="4">
         <v>45839</v>
@@ -785,7 +782,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3">
         <f>142*1000000</f>
@@ -799,16 +796,16 @@
         <v>1136000000</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I6" s="4">
         <v>45839</v>
@@ -823,6 +820,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="758ad4b0-59d6-43ba-9501-49561b83d908">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="758ad4b0-59d6-43ba-9501-49561b83d908" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca4bb2de-285c-40ff-aa89-c0d34fb084c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CA28BF95CB35104486B05271537623A7" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e35a3b96a2014548d4c2ecec0c4f4a64">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca4bb2de-285c-40ff-aa89-c0d34fb084c3" xmlns:ns3="758ad4b0-59d6-43ba-9501-49561b83d908" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="812fc3794f10ea3752c9bac50c43037e" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1074,36 +1100,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6568A05-A74A-4D5C-A968-212ACA36EB40}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="758ad4b0-59d6-43ba-9501-49561b83d908">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="758ad4b0-59d6-43ba-9501-49561b83d908" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca4bb2de-285c-40ff-aa89-c0d34fb084c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AFC672F-27C1-421C-B0AB-797CFC1AB694}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="758ad4b0-59d6-43ba-9501-49561b83d908"/>
+    <ds:schemaRef ds:uri="ca4bb2de-285c-40ff-aa89-c0d34fb084c3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96C7B366-607D-40DB-BF68-C0549239D843}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1123,26 +1140,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6568A05-A74A-4D5C-A968-212ACA36EB40}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AFC672F-27C1-421C-B0AB-797CFC1AB694}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="758ad4b0-59d6-43ba-9501-49561b83d908"/>
-    <ds:schemaRef ds:uri="ca4bb2de-285c-40ff-aa89-c0d34fb084c3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{1baa6d70-11a8-4c62-bb02-828ef39733af}" enabled="1" method="Standard" siteId="{3cd15905-3a8d-4330-a4fe-0ddaedc41022}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
new data update, formatting improvements
</commit_message>
<xml_diff>
--- a/public/risk.xlsx
+++ b/public/risk.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WesleyPowell\OneDrive - Scout Motors Inc\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EE0D77-2297-4496-AEBC-4462D3D76424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A389A927-099A-41E4-8F84-4D3178DB6E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5CE9F47-AF3C-47FC-B770-689BF2460523}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="risk" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">risk!$A$1:$I$14</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
+  <si>
+    <t>Likelihood</t>
+  </si>
+  <si>
+    <t>Risk x Likelihood</t>
+  </si>
+  <si>
+    <t>Responsible</t>
+  </si>
+  <si>
+    <t>Calculation Basis</t>
+  </si>
+  <si>
+    <t>Material costs worsen from May 2025 K-VAP status (VSI)</t>
+  </si>
+  <si>
+    <t>Target sales and service model not viable</t>
+  </si>
+  <si>
+    <t>Tariff risks on MEK from CAN, MEX, and EU sourcing</t>
+  </si>
+  <si>
+    <t>Tariff risks on production equipment and supplier tooling</t>
+  </si>
+  <si>
+    <t>Localization costs for LK4 and EA211 FSI</t>
+  </si>
+  <si>
+    <t>Lafrentz / Adam</t>
+  </si>
+  <si>
+    <t>Thacker / Sitron</t>
+  </si>
+  <si>
+    <t>Kodumudi</t>
+  </si>
+  <si>
+    <t>Kodumudi / Wollinsky</t>
+  </si>
   <si>
     <t>2027 - 2040</t>
   </si>
@@ -50,98 +92,123 @@
     <t>2027 - 2033</t>
   </si>
   <si>
+    <t>Material costs worsen from December 2024 K-VAP status (VSI)</t>
+  </si>
+  <si>
+    <t>Target sales and service model not viable </t>
+  </si>
+  <si>
+    <t>Battery system sourcing threatens cost versus December 2024 K-VAP status</t>
+  </si>
+  <si>
+    <t>Kodumudi / Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Factory commodity prices and supplier quotes above target versus December 2024 K-VAP status </t>
+  </si>
+  <si>
+    <t>Wollinsky</t>
+  </si>
+  <si>
+    <t>2023 - 2028</t>
+  </si>
+  <si>
+    <t>Scout’s environmental credit contribution to Group account is not as positive as PR74.SP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decker </t>
+  </si>
+  <si>
     <t>Risk Name</t>
   </si>
   <si>
     <t>Total Impact</t>
   </si>
   <si>
-    <t>Likelihood</t>
-  </si>
-  <si>
-    <t>Risk by Likelihood</t>
-  </si>
-  <si>
-    <t>Responsible</t>
-  </si>
-  <si>
     <t>Impact Years</t>
   </si>
   <si>
-    <t>Calculation Basis</t>
+    <t>$997 material cost decrease: $42,950 May  2025 K-VAP VSI vs $41,953 Aug. 2025 interim status;  Unrealized risk of $2,536 identified</t>
+  </si>
+  <si>
+    <t>Vehicle revenue loss from MSRP % paid to dealer; Loss of incremental revenues (parts, service, accessories, connectivity, and others); Other incremental costs (higher warranty cost provision, corporate OpEx, IT)</t>
+  </si>
+  <si>
+    <t>EA211: $157.3M initial invest + $57.7M for Silao expansion risk; LK4: $418.3M initial invest + $26.6M structure</t>
+  </si>
+  <si>
+    <t>LK4 imports from EU→Mexico; Non-USMCA compliant EDU assemblies; 15% duty on imported CKD components from EU; Battery cell imports for 2028 and early 2029</t>
+  </si>
+  <si>
+    <t>Equipment tariff and forex risk: $89.6M</t>
+  </si>
+  <si>
+    <t>$2,095 material cost increase; $42,950 May 2025 K-VAP VSI vs $40,855 Dec 2024 K-VAP VSI</t>
+  </si>
+  <si>
+    <t>10% battery system material cost increase vs December 2024 K-VAP VSI on 63 kWh EREV (10% increase on $4,107 battery system)</t>
+  </si>
+  <si>
+    <t>Sustained market feecback; 100% likelihood of $46M infrastructure risk compared to December 2024 K-VAP</t>
+  </si>
+  <si>
+    <t>Scout BEV installation rate decreased from 49% to 24% ; Trump administration likely to reduce targets. Additional mitigation measures will be derived as needed based on new regulations</t>
+  </si>
+  <si>
+    <t>Invest not accounted for in Group planning round; risk is considering NPV time effects</t>
+  </si>
+  <si>
+    <t>Sec. 232 tariffs on non-USA content for USMCA components has reduced in risk; IEEPA / Sec. 310 tariffs remain in effect on goods from China</t>
+  </si>
+  <si>
+    <t>Risk considers NPV time effects</t>
   </si>
   <si>
     <t>Updates</t>
   </si>
   <si>
+    <t>Material cost VSI improved since May 2025 K-VAP status due to Cost Sprint efforts; Risk identified in major components such as the battery pack based on supplier offers, LK4 prices, pre-assemblies and LV harnesses</t>
+  </si>
+  <si>
+    <t>Achieved licenses necessary to preserve go_x0002_to-market optionality in California, Missouri, Illinois, Utah – enabling 50-state direct sales; Arizona and Colorado license application underway, licenses expected Q3-Q4 2025; ~47 states open for direct service</t>
+  </si>
+  <si>
+    <t>Scout included invest in PR74.OP submission until agreement made by Group how funds should be accounted across Brands</t>
+  </si>
+  <si>
+    <t>Updated tariffs on imported auto parts from EU to 15%; Consider non-USMCA tariff risk of 27.5% on FR/RR EDUs w/Audi LK4 imports</t>
+  </si>
+  <si>
+    <t>Strategic pivot to remove 4x2 and make 4x4 standard across all trims; Further MEK reductions in preparation (e.g. entry ADAS, CMF optimizations, 12V battery, cost sprint)</t>
+  </si>
+  <si>
+    <t>Battery cell decision planned for May 27 K-VAP; Pack sourcing in progress with initial pack supplier quotes above VSI</t>
+  </si>
+  <si>
+    <t>Included in CapEx risk </t>
+  </si>
+  <si>
+    <t>EA211: $167M; LK4: $537M initial invest + $82M structure</t>
+  </si>
+  <si>
+    <t>Scout’s Range Extender considered as part of PR74.SP submission with 51% share; updated sales mix will be reflected in PR74.OP with 76% EREV share; Environmental credit implications to be calculated and consolidated at Group level</t>
+  </si>
+  <si>
+    <t>Based on C-Price tariff risk of $238/car on a palette basis on China, India, SK goods</t>
+  </si>
+  <si>
+    <t>Equipment tariff and forex risk:  $89.6M; Supplier tooling tariff risk:  $64.0M</t>
+  </si>
+  <si>
     <t>Date Added</t>
-  </si>
-  <si>
-    <t>Risk A</t>
-  </si>
-  <si>
-    <t>Risk B</t>
-  </si>
-  <si>
-    <t>Risk C</t>
-  </si>
-  <si>
-    <t>Risk D</t>
-  </si>
-  <si>
-    <t>Risk E</t>
-  </si>
-  <si>
-    <t>Responsible A</t>
-  </si>
-  <si>
-    <t>Responsible B</t>
-  </si>
-  <si>
-    <t>Responsible C</t>
-  </si>
-  <si>
-    <t>Responsible D</t>
-  </si>
-  <si>
-    <t>Responsible E</t>
-  </si>
-  <si>
-    <t>Calculation A</t>
-  </si>
-  <si>
-    <t>Calculation B</t>
-  </si>
-  <si>
-    <t>Calculation C</t>
-  </si>
-  <si>
-    <t>Calculation D</t>
-  </si>
-  <si>
-    <t>Calculation E</t>
-  </si>
-  <si>
-    <t>Update A</t>
-  </si>
-  <si>
-    <t>Update B</t>
-  </si>
-  <si>
-    <t>Update C</t>
-  </si>
-  <si>
-    <t>Update D</t>
-  </si>
-  <si>
-    <t>Update E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -187,7 +254,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -196,6 +263,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -206,56 +276,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -266,28 +292,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D55D8DBA-8FB4-4C67-9F9E-6DF313724C5F}" name="Table1" displayName="Table1" ref="A1:I6" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I6" xr:uid="{D55D8DBA-8FB4-4C67-9F9E-6DF313724C5F}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{BF13F786-4B04-4961-A30B-78983255055B}" name="Risk Name" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{B5D08A0D-A40D-4276-BB27-E84F502AEF02}" name="Total Impact" dataDxfId="7">
-      <calculatedColumnFormula>-1281*1000000</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{86BAB539-FD29-458F-B3C8-CA75E2D5E24F}" name="Likelihood" dataDxfId="6" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{44AB7870-F2B8-40F2-9B61-8A9C041484F9}" name="Risk by Likelihood" dataDxfId="5">
-      <calculatedColumnFormula>Table1[[#This Row],[Total Impact]]*Table1[[#This Row],[Likelihood]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{185EE216-6CE0-4433-8B49-A3D0EF80E5DE}" name="Responsible" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{2673E1ED-1064-4E6C-ABF7-D939B3437712}" name="Impact Years" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{CC3C2859-EFDE-405F-844A-58250EDF07DD}" name="Calculation Basis" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{B990CD74-FE9D-48EB-8B0D-51088C7BFC33}" name="Updates" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{43A2270C-CC3B-498C-9C65-628DB63036D8}" name="Date Added" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -606,251 +610,438 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B45BD30-AE42-4D8F-BD15-304F74FB6FD6}">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED1F689-0EF3-416B-960C-8636E2AA4822}">
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="46.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="171.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="204.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="46.109375" style="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>12</v>
+      <c r="A1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1281000000</v>
+      </c>
+      <c r="C2" s="1">
+        <v>85</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1088850000</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3">
-        <f>1281*1000000</f>
-        <v>1281000000</v>
-      </c>
-      <c r="C2" s="6">
-        <v>85</v>
-      </c>
-      <c r="D2" s="3">
-        <f>Table1[[#This Row],[Total Impact]]*Table1[[#This Row],[Likelihood]]</f>
-        <v>108885000000</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="4">
+      <c r="G2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="5">
         <v>45839</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3">
+        <v>8700000000</v>
+      </c>
+      <c r="C3" s="1">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1305000000</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3">
-        <f>8700*1000000</f>
-        <v>8700000000</v>
-      </c>
-      <c r="C3" s="6">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3">
-        <f>Table1[[#This Row],[Total Impact]]*Table1[[#This Row],[Likelihood]]</f>
-        <v>130500000000</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="4">
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="5">
         <v>45839</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>536000000</v>
+      </c>
+      <c r="C4" s="1">
+        <v>100</v>
+      </c>
+      <c r="D4" s="4">
+        <v>536000000</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3">
-        <f>536*1000000</f>
-        <v>536000000</v>
-      </c>
-      <c r="C4" s="6">
-        <v>100</v>
-      </c>
-      <c r="D4" s="3">
-        <f>Table1[[#This Row],[Total Impact]]*Table1[[#This Row],[Likelihood]]</f>
-        <v>53600000000</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="4">
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="5">
         <v>45839</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>382000000</v>
+      </c>
+      <c r="C5" s="1">
+        <v>80</v>
+      </c>
+      <c r="D5" s="4">
+        <v>305600000</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3">
-        <f>382*1000000</f>
-        <v>382000000</v>
-      </c>
-      <c r="C5" s="6">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3">
-        <f>Table1[[#This Row],[Total Impact]]*Table1[[#This Row],[Likelihood]]</f>
-        <v>3056000000</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="4">
+      <c r="G5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="5">
         <v>45839</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3">
+        <v>142000000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>80</v>
+      </c>
+      <c r="D6" s="4">
+        <v>113600000</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="5">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="3">
-        <f>142*1000000</f>
+      <c r="B7" s="3">
+        <v>1700000000</v>
+      </c>
+      <c r="C7" s="1">
+        <v>75</v>
+      </c>
+      <c r="D7" s="4">
+        <v>127500000000</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="5">
+        <v>45748</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3">
+        <v>8700000000</v>
+      </c>
+      <c r="C8" s="1">
+        <v>15</v>
+      </c>
+      <c r="D8" s="4">
+        <v>130500000000</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="5">
+        <v>45748</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3">
+        <v>342000000</v>
+      </c>
+      <c r="C9" s="1">
+        <v>60</v>
+      </c>
+      <c r="D9" s="4">
+        <v>20520000000</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="5">
+        <v>45748</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3">
+        <v>46000000</v>
+      </c>
+      <c r="C10" s="1">
+        <v>100</v>
+      </c>
+      <c r="D10" s="4">
+        <v>4600000000</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="5">
+        <v>45748</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3">
+        <v>609000000</v>
+      </c>
+      <c r="C11" s="1">
+        <v>100</v>
+      </c>
+      <c r="D11" s="4">
+        <v>60900000000</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="5">
+        <v>45748</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="1">
+        <v>100</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="5">
+        <v>45748</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3">
+        <v>198000000</v>
+      </c>
+      <c r="C13" s="1">
+        <v>80</v>
+      </c>
+      <c r="D13" s="4">
+        <v>15840000000</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="5">
+        <v>45748</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3">
         <v>142000000</v>
       </c>
-      <c r="C6" s="6">
-        <v>8</v>
-      </c>
-      <c r="D6" s="3">
-        <f>Table1[[#This Row],[Total Impact]]*Table1[[#This Row],[Likelihood]]</f>
-        <v>1136000000</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="4">
-        <v>45839</v>
+      <c r="C14" s="1">
+        <v>80</v>
+      </c>
+      <c r="D14" s="4">
+        <v>11360000000</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="5">
+        <v>45748</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I14" xr:uid="{1ED1F689-0EF3-416B-960C-8636E2AA4822}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="758ad4b0-59d6-43ba-9501-49561b83d908">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="758ad4b0-59d6-43ba-9501-49561b83d908" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca4bb2de-285c-40ff-aa89-c0d34fb084c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CA28BF95CB35104486B05271537623A7" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e35a3b96a2014548d4c2ecec0c4f4a64">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca4bb2de-285c-40ff-aa89-c0d34fb084c3" xmlns:ns3="758ad4b0-59d6-43ba-9501-49561b83d908" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="812fc3794f10ea3752c9bac50c43037e" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CA28BF95CB35104486B05271537623A7" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="65b4f997e36c2511eb5c7f6530ab6239">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca4bb2de-285c-40ff-aa89-c0d34fb084c3" xmlns:ns3="758ad4b0-59d6-43ba-9501-49561b83d908" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2de35c353c4288005d1e1d4e45c0faf" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="ca4bb2de-285c-40ff-aa89-c0d34fb084c3"/>
     <xsd:import namespace="758ad4b0-59d6-43ba-9501-49561b83d908"/>
@@ -1100,28 +1291,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6568A05-A74A-4D5C-A968-212ACA36EB40}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="758ad4b0-59d6-43ba-9501-49561b83d908">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="758ad4b0-59d6-43ba-9501-49561b83d908" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca4bb2de-285c-40ff-aa89-c0d34fb084c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AFC672F-27C1-421C-B0AB-797CFC1AB694}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="758ad4b0-59d6-43ba-9501-49561b83d908"/>
-    <ds:schemaRef ds:uri="ca4bb2de-285c-40ff-aa89-c0d34fb084c3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96C7B366-607D-40DB-BF68-C0549239D843}">
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30E47FE2-4884-4216-B41C-A8256015DAE6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -1140,6 +1340,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AFC672F-27C1-421C-B0AB-797CFC1AB694}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="758ad4b0-59d6-43ba-9501-49561b83d908"/>
+    <ds:schemaRef ds:uri="ca4bb2de-285c-40ff-aa89-c0d34fb084c3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6568A05-A74A-4D5C-A968-212ACA36EB40}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{1baa6d70-11a8-4c62-bb02-828ef39733af}" enabled="1" method="Standard" siteId="{3cd15905-3a8d-4330-a4fe-0ddaedc41022}" contentBits="0" removed="0"/>

</xml_diff>